<commit_message>
Implement GAAP Reasoning Logic for ambiguous items
</commit_message>
<xml_diff>
--- a/Excel Templates/balance_sheet/Basic_Style/StatementXL_Balance_Sheet_Template_Basic_XLSX.xlsx
+++ b/Excel Templates/balance_sheet/Basic_Style/StatementXL_Balance_Sheet_Template_Basic_XLSX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Desktop\StatementXL_Version_2\Excel Templates\balance_sheet\Basic_Style\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4E87C49-4577-4EAF-BE27-4041424EE366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68282564-4C07-4D42-925A-3FAFDC683937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Balance Sheet</t>
   </si>
@@ -41,10 +41,118 @@
     <t>Line Items</t>
   </si>
   <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Current Assets</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Other Current Assets</t>
+  </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>Non-Current Assets</t>
+  </si>
+  <si>
+    <t>Other Non-Current Assets</t>
+  </si>
+  <si>
+    <t>Total Non-Current Assets</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>Current Liabilities</t>
+  </si>
+  <si>
+    <t>Accounts Payable</t>
+  </si>
+  <si>
+    <t>Accrued Expenses</t>
+  </si>
+  <si>
+    <t>Short-Term Debt</t>
+  </si>
+  <si>
+    <t>Total Current Liabilities</t>
+  </si>
+  <si>
+    <t>Non-Current Liabilities</t>
+  </si>
+  <si>
+    <t>Long-Term Debt</t>
+  </si>
+  <si>
+    <t>Deferred Tax Liabilities</t>
+  </si>
+  <si>
+    <t>Total Non-Current Liabilities</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>Common Stock</t>
+  </si>
+  <si>
+    <t>Retained Earnings</t>
+  </si>
+  <si>
+    <t>Accumulated Other Comprehensive Income</t>
+  </si>
+  <si>
     <t>"Company Name"</t>
   </si>
   <si>
     <t>Year(s) Ended</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts Receivable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepaid Expenses </t>
+  </si>
+  <si>
+    <t>Plant, Property &amp; Equipment</t>
+  </si>
+  <si>
+    <t>Intangible Assets, Net</t>
+  </si>
+  <si>
+    <t>Goodwill</t>
+  </si>
+  <si>
+    <t>Deferred Revenue</t>
+  </si>
+  <si>
+    <t>Total Assests</t>
+  </si>
+  <si>
+    <t>Other Long-Term Liabilities</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Additional Paid-in-Capital</t>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t>Total Liabilities &amp; Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Balance Check</t>
   </si>
 </sst>
 </file>
@@ -102,7 +210,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,13 +219,14 @@
     </font>
     <font>
       <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,12 +271,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FF1F4E79"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -232,30 +372,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -270,66 +386,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,124 +401,178 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="4" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="22">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="8" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
@@ -767,177 +884,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK57" sqref="AK57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="2.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="C5" s="23">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5">
+        <f>SUM(C8:C12)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+    </row>
+    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5">
+        <f>SUM(C17:C20)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5">
+        <f>C13+C21</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="18"/>
+    </row>
+    <row r="26" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="28"/>
+    </row>
+    <row r="27" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5">
+        <f>SUM(C28:C31)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+    </row>
+    <row r="34" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="17"/>
+    </row>
+    <row r="35" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+    </row>
+    <row r="36" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="5">
+        <f>SUM(C36:C38)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="25"/>
+    </row>
+    <row r="41" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="5">
+        <f>C32+C39</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="20"/>
+      <c r="C42" s="25"/>
+    </row>
+    <row r="43" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="19"/>
+    </row>
+    <row r="44" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="20"/>
+      <c r="C44" s="25"/>
+    </row>
+    <row r="45" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="32">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="33">
+        <f>SUM(C45:C48)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="20"/>
+      <c r="C50" s="25"/>
+    </row>
+    <row r="51" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="33">
+        <f>C41+C49</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="20"/>
+      <c r="C52" s="25"/>
+    </row>
+    <row r="53" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="30">
+        <f>C23-C51</f>
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="25"/>
-      <c r="C16" s="20"/>
-    </row>
-    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-    </row>
-    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-    </row>
-    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-    </row>
-    <row r="21" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
-    </row>
-    <row r="22" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-    </row>
-    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-    </row>
-    <row r="24" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-    </row>
-    <row r="25" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="34"/>
-    </row>
-    <row r="26" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="38"/>
-      <c r="C26" s="36"/>
-    </row>
-    <row r="27" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="28"/>
-    </row>
-    <row r="28" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-    </row>
-    <row r="29" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="41"/>
-      <c r="C29" s="42"/>
-    </row>
-    <row r="30" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
-    </row>
-    <row r="31" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="25"/>
-      <c r="C31" s="20"/>
-    </row>
-    <row r="32" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="26"/>
-      <c r="C32" s="18"/>
-    </row>
-    <row r="33" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-    </row>
-    <row r="34" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
-      <c r="C34" s="15"/>
-    </row>
-    <row r="35" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="26"/>
-      <c r="C35" s="18"/>
-    </row>
+    </row>
+    <row r="54" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:XFD8 A13:XFD14 A21:XFD22 A29:XFD29 A34:XFD34">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="A13:A14 A22:A23 A29 A34 A7:A8 B8:B9 D13:XFD14 D22:XFD23 D29:XFD29 D34:XFD34 C7:XFD7 D8:XFD8">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:XFD9 A15:XFD15 A17:XFD17 A23:XFD23 A25:XFD25 A30:XFD30 A35:XFD35 G37">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="G37 A9 A15:A16 A18 A24 A30 A35 D9:XFD9 D15:XFD16 D18:XFD18 D24:XFD24 D30:XFD30 D35:XFD35">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C12">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:C20">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C31">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:C38">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:C48">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13 C23 C21 C32 C39 C41 C49 C51">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47 A8:XFD12 A17:XFD20 A28:XFD31 A36:XFD38">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J50 A53:XFD53 A51:XFD51 A49:XFD49 A41:XFD41 A39:XFD39 A32:XFD32 A23:XFD23 A21:XFD21 A13:XFD13">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>